<commit_message>
New Commit with Thread Local Implementation .
</commit_message>
<xml_diff>
--- a/data/TC002.xlsx
+++ b/data/TC002.xlsx
@@ -57,22 +57,22 @@
     <t>Testing3</t>
   </si>
   <si>
-    <t>Mathan73</t>
-  </si>
-  <si>
-    <t>Mathan74</t>
-  </si>
-  <si>
-    <t>Mathan75</t>
-  </si>
-  <si>
-    <t>mathan73@gmail.com</t>
-  </si>
-  <si>
-    <t>mathan74@gmail.com</t>
-  </si>
-  <si>
-    <t>mathan75@gmail.com</t>
+    <t>Mathan90</t>
+  </si>
+  <si>
+    <t>Mathan91</t>
+  </si>
+  <si>
+    <t>Mathan92</t>
+  </si>
+  <si>
+    <t>mathan90@gmail.com</t>
+  </si>
+  <si>
+    <t>mathan91@gmail.com</t>
+  </si>
+  <si>
+    <t>mathan92@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>